<commit_message>
fixing data and model
</commit_message>
<xml_diff>
--- a/model/resources/config.xlsx
+++ b/model/resources/config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>א</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>ֻּ</t>
+  </si>
+  <si>
+    <t>ץ</t>
+  </si>
+  <si>
+    <t>ץ'</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
   </si>
 </sst>
 </file>
@@ -553,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A23" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A28" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -893,6 +905,26 @@
         <v>32</v>
       </c>
     </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>